<commit_message>
add looping for many passengers
</commit_message>
<xml_diff>
--- a/Data Collection/Data_Management_.xlsx
+++ b/Data Collection/Data_Management_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afrizaloky\Katalon Studio\Assignment Katalon\Data Collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFBF66F-96F2-4569-B89A-5E78975A78D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA268B7-2AB0-4E09-A3F7-04A2E646AE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="158">
   <si>
     <t>Title</t>
   </si>
@@ -491,6 +491,12 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>Alim-mimi</t>
+  </si>
+  <si>
+    <t>Mr-Mrs-Mr-Ms</t>
   </si>
 </sst>
 </file>
@@ -3000,7 +3006,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3086,7 +3092,7 @@
     </row>
     <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>145</v>
@@ -3127,7 +3133,7 @@
         <v>134</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
create test case for all
</commit_message>
<xml_diff>
--- a/Data Collection/Data_Management_.xlsx
+++ b/Data Collection/Data_Management_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afrizaloky\Katalon Studio\Assignment Katalon\Data Collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B98CB3-85BE-4379-957E-1C1D1EBD38F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A0FBDA-5721-4647-9678-4BA667E380E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="175">
   <si>
     <t>Title</t>
   </si>
@@ -848,7 +848,7 @@
   <dimension ref="A1:L995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:K32"/>
+      <selection activeCell="L1" sqref="L1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3226,7 +3226,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3295,8 +3295,23 @@
       <c r="T1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" s="5" t="s">
-        <v>1</v>
+      <c r="U1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
@@ -3360,8 +3375,23 @@
       <c r="T2" s="2">
         <v>0</v>
       </c>
-      <c r="Z2" s="5" t="s">
-        <v>6</v>
+      <c r="U2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>8798132</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.25">
@@ -3425,8 +3455,23 @@
       <c r="T3" s="2">
         <v>0</v>
       </c>
-      <c r="Z3" s="5" t="s">
-        <v>6</v>
+      <c r="U3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>2121121</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.25">
@@ -3490,8 +3535,23 @@
       <c r="T4" s="2">
         <v>0</v>
       </c>
-      <c r="Z4" s="5" t="s">
-        <v>6</v>
+      <c r="U4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>12122121</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.25">
@@ -3555,8 +3615,23 @@
       <c r="T5" s="2">
         <v>0</v>
       </c>
-      <c r="Z5" s="5" t="s">
-        <v>6</v>
+      <c r="U5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>11212111</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -4739,7 +4814,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>